<commit_message>
Updated code in excel download, import and probation
</commit_message>
<xml_diff>
--- a/ExcelTemplates/Bulk Leave Application Import.xlsx
+++ b/ExcelTemplates/Bulk Leave Application Import.xlsx
@@ -1,31 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\internship041\source\repos\BackendAttendance\ExcelTemplates\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C4084F7-7036-4480-997B-939AE3C18D19}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28908"/>
+  <workbookPr/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D5D33A68-E1D7-4C02-8E50-997155503D22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" xr2:uid="{F1726B7F-C878-4AAD-93B0-34652856F6EC}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>StaffId</t>
   </si>
@@ -36,10 +42,7 @@
     <t>EndDuration</t>
   </si>
   <si>
-    <t>ApplicationTypeName</t>
-  </si>
-  <si>
-    <t>LeaveTypeName</t>
+    <t>LeaveType</t>
   </si>
   <si>
     <t>FromDate</t>
@@ -48,33 +51,24 @@
     <t>ToDate</t>
   </si>
   <si>
+    <t>TotalDays</t>
+  </si>
+  <si>
     <t>Reason</t>
   </si>
   <si>
-    <t>VL12</t>
-  </si>
-  <si>
-    <t>Earned Leave</t>
-  </si>
-  <si>
-    <t>Full Day</t>
-  </si>
-  <si>
-    <t>Fever</t>
-  </si>
-  <si>
-    <t>Leave Requisition</t>
+    <t>ApplicationType</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -99,15 +93,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -130,39 +125,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="0E2841"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="E8E8E8"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="145F82"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="E87331"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="186C24"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="0F9ED5"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="A02B93"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="4EA72E"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="467886"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="96607D"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Aptos Display" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -214,7 +209,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -325,13 +320,6 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -340,6 +328,13 @@
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -404,7 +399,27 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
@@ -415,75 +430,60 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D3CD4E4-0D7A-4D69-ADD9-886FA8FCD720}">
-  <dimension ref="A1:H2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
-    <col min="5" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
-        <v>3</v>
+      <c r="I1" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="1">
-        <v>45628</v>
-      </c>
-      <c r="F2" s="1">
-        <v>45631</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" t="s">
-        <v>12</v>
-      </c>
+    <row r="2" spans="1:15">
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="M2" s="2"/>
+      <c r="O2" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>